<commit_message>
related work about kg
</commit_message>
<xml_diff>
--- a/知识图谱/content.xlsx
+++ b/知识图谱/content.xlsx
@@ -1,86 +1,130 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\实验室相关\人机物\论文\RelatedWorks\软件定义建模与执行\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37825D21-3B63-444D-BF7A-6592D2DE7FC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="223" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="223"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>First Author</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
   <si>
     <t>Reactive Microservices for the Internet of Things: A case study in Fog Computing</t>
   </si>
   <si>
-    <t>Title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Year</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Abstract</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>C. de Santana</t>
+  </si>
+  <si>
+    <t>The Future Internet will be able to connect most of the objects that are not yet connected on the current Internet. The Internet of Things (IoT) is an important part of the Future Internet and involves connectivity between several physical and virtual objects, allowing the emergence of new services and applications. These intelligent objects, along with their tasks, constitute domain-specific applications (vertical markets), while ubiquitous and analytic services form independent domain services (horizontal markets). The development of these applications and services in these markets brings challenges such as deployment, scalability, integration, interoperability, mobility and performance. Recent research indicates that Microservices has been successfully applied by companies such as Netflix and SoundCloud to address some of these issues in their cloud computing applications. However, in the field of IoT, the use of Microservices to deal with these challenges still presents unresolved issues. In this paper, we present a reactive Microservices architecture and apply it in a Fog Computing case study to investigate these challenges at the edge of the network. Finally, we evaluate our proposal from the perspective of performance of Microservices provided by intelligent objects (IoT gateways) at the edge of the network.</t>
   </si>
   <si>
     <t>https://dl.acm.org/doi/10.1145/3297280.3297402</t>
   </si>
   <si>
-    <t>Ind</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Link</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Future Internet will be able to connect most of the objects that are not yet connected on the current Internet. The Internet of Things (IoT) is an important part of the Future Internet and involves connectivity between several physical and virtual objects, allowing the emergence of new services and applications. These intelligent objects, along with their tasks, constitute domain-specific applications (vertical markets), while ubiquitous and analytic services form independent domain services (horizontal markets). The development of these applications and services in these markets brings challenges such as deployment, scalability, integration, interoperability, mobility and performance. Recent research indicates that Microservices has been successfully applied by companies such as Netflix and SoundCloud to address some of these issues in their cloud computing applications. However, in the field of IoT, the use of Microservices to deal with these challenges still presents unresolved issues. In this paper, we present a reactive Microservices architecture and apply it in a Fog Computing case study to investigate these challenges at the edge of the network. Finally, we evaluate our proposal from the perspective of performance of Microservices provided by intelligent objects (IoT gateways) at the edge of the network.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C. de Santana</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>First Author</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Runtime knowledge graph based approach to smart home application development</t>
+  </si>
+  <si>
+    <t>Minchen Zhu</t>
+  </si>
+  <si>
+    <t>Smart home is an important application area of the Internet of things (IoT). However, the diversification of smart home application scenarios increases the difficulty of 
+understanding the scenarios for developers. And the heterogeneity of the programming interfaces of smart devices as well as the close coupling of the code to the underlying systems is still an important work for the developers. Furthermore, the complexity and variability of business requirements poses a great challenge to the development of  applications logic. In this paper, we present a runtime knowledge graph based approach to smart home application development. First, a conceptual model describing the smart home scenarios is defined. Second, the manageability of smart devices is abstracted as runtime knowledge graphs that are automatically connected with the corresponding systems. Last, a method of automatically generating smart home applications is proposed. Our approach can reduce code by about 85 percent at least, and an experiment on a real-world application scenario demonstrates the feasibility, effectiveness, and benefits of the new approach to smart home application development.</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/8473447</t>
+  </si>
+  <si>
+    <t>A3ID: An Automatic and Interpretable ImplicitInterference Detection Method for Smart Home via Knowledge Graph</t>
+  </si>
+  <si>
+    <t>Ding Xiao</t>
+  </si>
+  <si>
+    <r>
+      <t>The smart home brings together devices, the cloud,data, and people to make home living more comfortable and safer. Trigger–action programming enables users to connect smart devices using if-this-then-that (IFTTT)-style rules. Withthe increasing number of devices in smart home systems, multiple running rules that act on actuators in contradictory ways may cause unexpected and unpredictable interference problems,which can put residents and their belongings at risk. Previous studies have considered explicit interference problems related to multiple rules targeting a single actuator, whereas implicit interference (interference across different actuators) detection is still challenging and not yet well studied owing to the effort</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>x0002_intensive and time-consuming annotation work of obtaining device information. The lack of knowledge about devices is a critical reason that affects the accuracy and efficiency in implicit interference detection. In this article, we propose A3ID, an automatic detection method for implicit interference based
+on knowledge graphs. Using natural language processing (NLP) techniques and a lexical database, A3ID can extract knowledge of devices from a knowledge graph, including functionality, effect, and scope. Then, it analyzes and detects interferences among the different devices semantically in three steps, without human intervention. Furthermore, it provides user-friendly explanations in a well-designed structure to specify possible reasons for the implicit interference problems. Our experiment on 11 859</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="134"/>
+      </rPr>
+      <t>IFTTT_x0002_style rules shows that A3ID outperforms state-of-the-art methods by more than 33% in the F1-score for the detection of implicit interference. Moreover, evaluations on an extended data set for devices from ConceptNet (a knowledge graph) and five smart home systems suggest that A3ID also has favorable performance with other devices not limited to the smart home domain.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/8930944</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -88,24 +132,367 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -113,37 +500,331 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +873,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -227,7 +908,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -401,83 +1082,116 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="1"/>
-    <col min="2" max="2" width="67.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.73046875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="176.3984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.53125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.06640625" style="1"/>
+    <col min="1" max="1" width="9.06481481481481" style="1"/>
+    <col min="2" max="2" width="67.6018518518518" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7962962962963" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.73148148148148" style="1" customWidth="1"/>
+    <col min="5" max="5" width="176.398148148148" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.5277777777778" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.06481481481481" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.4" x14ac:dyDescent="0.4">
+    <row r="1" ht="15.6" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" ht="93" customHeight="1" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>2019</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C3" s="3"/>
+    <row r="3" ht="82.8" spans="1:6">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2018</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C4" s="3"/>
+    <row r="4" ht="138" spans="1:6">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="https://ieeexplore.ieee.org/document/8473447"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://ieeexplore.ieee.org/document/8930944"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>